<commit_message>
Fix sign in treatment datasets for vanadium battery
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-batteries-vanadium-redox-flow.xlsx
+++ b/premise/data/additional_inventories/lci-batteries-vanadium-redox-flow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahnme_a\PycharmProjects\premise\premise\data\additional_inventories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D8E722-F53E-49DE-8C0D-6DADE6074A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFD2C97-861D-1F45-942B-B18D3E09D009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{26241F67-8618-094B-AD38-E491C9570B84}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" xr2:uid="{26241F67-8618-094B-AD38-E491C9570B84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1275,7 +1275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1286,7 +1286,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1305,9 +1304,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1345,7 +1344,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1451,7 +1450,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1593,7 +1592,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1603,21 +1602,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1C5B3A-29A3-3D4D-87B5-E2283E6AD55F}">
   <dimension ref="A1:P475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
-      <selection activeCell="B459" sqref="B459"/>
+    <sheetView tabSelected="1" topLeftCell="A446" workbookViewId="0">
+      <selection activeCell="B472" sqref="B472"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="63" customWidth="1"/>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.375" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1625,7 +1624,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1636,7 +1635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1647,7 +1646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1658,7 +1657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1666,7 +1665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1674,7 +1673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1685,7 +1684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1696,7 +1695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1715,7 +1714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1741,7 +1740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1761,7 +1760,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1791,7 +1790,7 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -1818,7 +1817,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -1843,7 +1842,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>277</v>
       </c>
@@ -1868,7 +1867,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>279</v>
       </c>
@@ -1893,7 +1892,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
@@ -1918,7 +1917,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>281</v>
       </c>
@@ -1943,7 +1942,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>282</v>
       </c>
@@ -1968,7 +1967,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>284</v>
       </c>
@@ -1993,7 +1992,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>286</v>
       </c>
@@ -2017,7 +2016,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>276</v>
       </c>
@@ -2041,7 +2040,7 @@
       <c r="K24" s="4"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>55</v>
       </c>
@@ -2067,7 +2066,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -2093,7 +2092,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>288</v>
       </c>
@@ -2122,7 +2121,7 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>289</v>
       </c>
@@ -2151,7 +2150,7 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>291</v>
       </c>
@@ -2180,13 +2179,13 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -2208,7 +2207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -2219,7 +2218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2227,7 +2226,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2246,7 +2245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -2257,7 +2256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2268,7 +2267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
@@ -2302,7 +2301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f>B31</f>
         <v>polyacrylonitrile-based electrode production, for VRFB system</v>
@@ -2325,7 +2324,7 @@
       </c>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>292</v>
       </c>
@@ -2352,7 +2351,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>282</v>
       </c>
@@ -2379,7 +2378,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>282</v>
       </c>
@@ -2406,7 +2405,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>338</v>
       </c>
@@ -2433,7 +2432,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>50</v>
       </c>
@@ -2454,7 +2453,7 @@
       </c>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>65</v>
       </c>
@@ -2478,7 +2477,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>66</v>
       </c>
@@ -2503,13 +2502,13 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>1</v>
       </c>
@@ -2520,7 +2519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -2531,7 +2530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2569,7 +2568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>9</v>
       </c>
@@ -2580,7 +2579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -2591,7 +2590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>12</v>
       </c>
@@ -2599,7 +2598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>13</v>
       </c>
@@ -2625,7 +2624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f>B50</f>
         <v>bipolar plate production, for VRFB system</v>
@@ -2648,7 +2647,7 @@
       </c>
       <c r="I60" s="4"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>86</v>
       </c>
@@ -2675,7 +2674,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>210</v>
       </c>
@@ -2702,7 +2701,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>87</v>
       </c>
@@ -2729,7 +2728,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>88</v>
       </c>
@@ -2756,7 +2755,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>340</v>
       </c>
@@ -2783,7 +2782,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>89</v>
       </c>
@@ -2810,7 +2809,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>90</v>
       </c>
@@ -2837,7 +2836,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>322</v>
       </c>
@@ -2864,7 +2863,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>342</v>
       </c>
@@ -2891,7 +2890,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>91</v>
       </c>
@@ -2918,7 +2917,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>282</v>
       </c>
@@ -2945,7 +2944,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>282</v>
       </c>
@@ -2972,7 +2971,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>358</v>
       </c>
@@ -2999,7 +2998,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>344</v>
       </c>
@@ -3026,7 +3025,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>286</v>
       </c>
@@ -3053,7 +3052,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>289</v>
       </c>
@@ -3077,13 +3076,13 @@
       </c>
       <c r="I76" s="4"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>1</v>
       </c>
@@ -3094,7 +3093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -3105,7 +3104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -3116,7 +3115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -3124,7 +3123,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -3132,7 +3131,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -3143,7 +3142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>9</v>
       </c>
@@ -3154,7 +3153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -3165,7 +3164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>12</v>
       </c>
@@ -3173,7 +3172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>13</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
         <f>B78</f>
         <v>stack frame assembly, for VRFB system</v>
@@ -3222,7 +3221,7 @@
       </c>
       <c r="I88" s="4"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>109</v>
       </c>
@@ -3249,7 +3248,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>346</v>
       </c>
@@ -3276,7 +3275,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>110</v>
       </c>
@@ -3303,7 +3302,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>344</v>
       </c>
@@ -3330,7 +3329,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>286</v>
       </c>
@@ -3357,7 +3356,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>1</v>
       </c>
@@ -3368,7 +3367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>3</v>
       </c>
@@ -3379,7 +3378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -3390,7 +3389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -3398,7 +3397,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -3406,7 +3405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -3417,7 +3416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -3428,7 +3427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -3439,7 +3438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>12</v>
       </c>
@@ -3447,7 +3446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>13</v>
       </c>
@@ -3473,7 +3472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="str">
         <f>B95</f>
         <v>vanadium electrolyte solution production</v>
@@ -3499,7 +3498,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>122</v>
       </c>
@@ -3526,7 +3525,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>120</v>
       </c>
@@ -3553,7 +3552,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>348</v>
       </c>
@@ -3580,7 +3579,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>342</v>
       </c>
@@ -3607,7 +3606,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>344</v>
       </c>
@@ -3634,7 +3633,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>286</v>
       </c>
@@ -3661,7 +3660,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>350</v>
       </c>
@@ -3688,7 +3687,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>352</v>
       </c>
@@ -3715,7 +3714,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>284</v>
       </c>
@@ -3738,7 +3737,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>1</v>
       </c>
@@ -3749,7 +3748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>3</v>
       </c>
@@ -3760,7 +3759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>5</v>
       </c>
@@ -3771,7 +3770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3779,7 +3778,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>7</v>
       </c>
@@ -3787,7 +3786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -3798,7 +3797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>9</v>
       </c>
@@ -3809,7 +3808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -3820,7 +3819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>12</v>
       </c>
@@ -3828,7 +3827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>13</v>
       </c>
@@ -3854,7 +3853,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="str">
         <f>B116</f>
         <v>electrolyte tank production, for VRFB system</v>
@@ -3880,7 +3879,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>130</v>
       </c>
@@ -3904,7 +3903,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>332</v>
       </c>
@@ -3928,7 +3927,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>131</v>
       </c>
@@ -3952,7 +3951,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>354</v>
       </c>
@@ -3976,7 +3975,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>158</v>
       </c>
@@ -4000,7 +3999,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>286</v>
       </c>
@@ -4027,7 +4026,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>344</v>
       </c>
@@ -4051,7 +4050,7 @@
       <c r="K133" s="3"/>
       <c r="L133" s="3"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>350</v>
       </c>
@@ -4075,7 +4074,7 @@
       <c r="K134" s="3"/>
       <c r="L134" s="3"/>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>336</v>
       </c>
@@ -4096,7 +4095,7 @@
       </c>
       <c r="I135" s="4"/>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>129</v>
       </c>
@@ -4117,13 +4116,13 @@
       <c r="K136" s="3"/>
       <c r="L136" s="3"/>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
       <c r="K137" s="3"/>
       <c r="L137" s="3"/>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>1</v>
       </c>
@@ -4134,7 +4133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>3</v>
       </c>
@@ -4145,7 +4144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>5</v>
       </c>
@@ -4156,7 +4155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>6</v>
       </c>
@@ -4164,7 +4163,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>7</v>
       </c>
@@ -4172,7 +4171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>8</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -4194,7 +4193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>11</v>
       </c>
@@ -4205,7 +4204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>12</v>
       </c>
@@ -4213,7 +4212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>13</v>
       </c>
@@ -4240,7 +4239,7 @@
       </c>
       <c r="I147" s="4"/>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" t="str">
         <f>B138</f>
         <v>current collector production, for VRFB system</v>
@@ -4266,7 +4265,7 @@
       <c r="K148" s="3"/>
       <c r="L148" s="3"/>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>324</v>
       </c>
@@ -4293,7 +4292,7 @@
       <c r="K149" s="3"/>
       <c r="L149" s="3"/>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>141</v>
       </c>
@@ -4320,7 +4319,7 @@
       <c r="K150" s="3"/>
       <c r="L150" s="3"/>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>356</v>
       </c>
@@ -4347,7 +4346,7 @@
       <c r="K151" s="3"/>
       <c r="L151" s="3"/>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>344</v>
       </c>
@@ -4374,7 +4373,7 @@
       <c r="K152" s="3"/>
       <c r="L152" s="3"/>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>286</v>
       </c>
@@ -4398,13 +4397,13 @@
       </c>
       <c r="I153" s="4"/>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
       <c r="L154" s="3"/>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>1</v>
       </c>
@@ -4415,7 +4414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>3</v>
       </c>
@@ -4426,7 +4425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>5</v>
       </c>
@@ -4437,7 +4436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>6</v>
       </c>
@@ -4445,7 +4444,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>7</v>
       </c>
@@ -4453,7 +4452,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>8</v>
       </c>
@@ -4464,7 +4463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>9</v>
       </c>
@@ -4475,7 +4474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>11</v>
       </c>
@@ -4486,7 +4485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>12</v>
       </c>
@@ -4494,7 +4493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>13</v>
       </c>
@@ -4521,7 +4520,7 @@
       </c>
       <c r="I164" s="4"/>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="str">
         <f>B155</f>
         <v>polyvinylchloride cell frame production, for VRFB system</v>
@@ -4544,7 +4543,7 @@
       </c>
       <c r="I165" s="4"/>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>354</v>
       </c>
@@ -4569,7 +4568,7 @@
       <c r="K166" s="3"/>
       <c r="L166" s="3"/>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>158</v>
       </c>
@@ -4594,7 +4593,7 @@
       <c r="K167" s="3"/>
       <c r="L167" s="3"/>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>286</v>
       </c>
@@ -4619,7 +4618,7 @@
       <c r="K168" s="3"/>
       <c r="L168" s="3"/>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>344</v>
       </c>
@@ -4644,7 +4643,7 @@
       <c r="K169" s="3"/>
       <c r="L169" s="3"/>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>1</v>
       </c>
@@ -4655,7 +4654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>3</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>5</v>
       </c>
@@ -4677,7 +4676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>6</v>
       </c>
@@ -4685,7 +4684,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>7</v>
       </c>
@@ -4693,7 +4692,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>8</v>
       </c>
@@ -4704,7 +4703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>9</v>
       </c>
@@ -4715,7 +4714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>11</v>
       </c>
@@ -4726,7 +4725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>12</v>
       </c>
@@ -4734,7 +4733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>13</v>
       </c>
@@ -4761,7 +4760,7 @@
       </c>
       <c r="I180" s="4"/>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="str">
         <f>B171</f>
         <v>gasket production, FKM, for VRFB system</v>
@@ -4783,7 +4782,7 @@
         <v>gasket, FKM</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>156</v>
       </c>
@@ -4806,7 +4805,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>157</v>
       </c>
@@ -4829,7 +4828,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
         <v>334</v>
       </c>
@@ -4852,7 +4851,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>158</v>
       </c>
@@ -4875,7 +4874,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
         <v>286</v>
       </c>
@@ -4898,7 +4897,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>344</v>
       </c>
@@ -4921,7 +4920,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>1</v>
       </c>
@@ -4932,7 +4931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>3</v>
       </c>
@@ -4943,7 +4942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>5</v>
       </c>
@@ -4954,7 +4953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>6</v>
       </c>
@@ -4962,7 +4961,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>7</v>
       </c>
@@ -4970,7 +4969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>8</v>
       </c>
@@ -4981,7 +4980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>9</v>
       </c>
@@ -4992,7 +4991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>11</v>
       </c>
@@ -5003,7 +5002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>12</v>
       </c>
@@ -5011,7 +5010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>13</v>
       </c>
@@ -5038,7 +5037,7 @@
       </c>
       <c r="I198" s="4"/>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="str">
         <f>B189</f>
         <v>copper cable production, for VRFB system</v>
@@ -5060,7 +5059,7 @@
         <v>copper cable, for VRFB system</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
         <v>167</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
         <v>324</v>
       </c>
@@ -5106,7 +5105,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>354</v>
       </c>
@@ -5129,7 +5128,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>321</v>
       </c>
@@ -5152,7 +5151,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>158</v>
       </c>
@@ -5175,7 +5174,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>320</v>
       </c>
@@ -5198,7 +5197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
         <v>344</v>
       </c>
@@ -5221,7 +5220,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>286</v>
       </c>
@@ -5244,7 +5243,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>330</v>
       </c>
@@ -5267,7 +5266,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
         <v>289</v>
       </c>
@@ -5290,7 +5289,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
         <v>77</v>
       </c>
@@ -5311,7 +5310,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>77</v>
       </c>
@@ -5331,7 +5330,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>1</v>
       </c>
@@ -5342,7 +5341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>3</v>
       </c>
@@ -5353,7 +5352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>5</v>
       </c>
@@ -5364,7 +5363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>6</v>
       </c>
@@ -5372,7 +5371,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>7</v>
       </c>
@@ -5380,7 +5379,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>8</v>
       </c>
@@ -5391,7 +5390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>9</v>
       </c>
@@ -5402,7 +5401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>11</v>
       </c>
@@ -5413,7 +5412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>12</v>
       </c>
@@ -5421,7 +5420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>13</v>
       </c>
@@ -5448,7 +5447,7 @@
       </c>
       <c r="I222" s="4"/>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223" t="str">
         <f>B213</f>
         <v>pumps assembly, for VRFB system</v>
@@ -5474,7 +5473,7 @@
       <c r="K223" s="3"/>
       <c r="L223" s="3"/>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
         <v>328</v>
       </c>
@@ -5501,7 +5500,7 @@
       <c r="K224" s="3"/>
       <c r="L224" s="3"/>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>176</v>
       </c>
@@ -5528,7 +5527,7 @@
       <c r="K225" s="3"/>
       <c r="L225" s="3"/>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
         <v>324</v>
       </c>
@@ -5555,7 +5554,7 @@
       <c r="K226" s="3"/>
       <c r="L226" s="3"/>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>354</v>
       </c>
@@ -5582,7 +5581,7 @@
       <c r="K227" s="3"/>
       <c r="L227" s="3"/>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
         <v>326</v>
       </c>
@@ -5609,7 +5608,7 @@
       <c r="K228" s="3"/>
       <c r="L228" s="3"/>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>319</v>
       </c>
@@ -5636,7 +5635,7 @@
       <c r="K229" s="3"/>
       <c r="L229" s="3"/>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
         <v>318</v>
       </c>
@@ -5663,7 +5662,7 @@
       <c r="K230" s="3"/>
       <c r="L230" s="3"/>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
         <v>317</v>
       </c>
@@ -5690,7 +5689,7 @@
       <c r="K231" s="3"/>
       <c r="L231" s="3"/>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
         <v>344</v>
       </c>
@@ -5717,7 +5716,7 @@
       <c r="K232" s="3"/>
       <c r="L232" s="3"/>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
         <v>286</v>
       </c>
@@ -5741,7 +5740,7 @@
       </c>
       <c r="I233" s="4"/>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
         <v>289</v>
       </c>
@@ -5768,7 +5767,7 @@
       <c r="K234" s="3"/>
       <c r="L234" s="3"/>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
         <v>311</v>
       </c>
@@ -5795,13 +5794,13 @@
       <c r="K235" s="3"/>
       <c r="L235" s="3"/>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I236" s="3"/>
       <c r="J236" s="3"/>
       <c r="K236" s="3"/>
       <c r="L236" s="3"/>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>1</v>
       </c>
@@ -5812,7 +5811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>3</v>
       </c>
@@ -5823,7 +5822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>5</v>
       </c>
@@ -5834,7 +5833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>6</v>
       </c>
@@ -5842,7 +5841,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>7</v>
       </c>
@@ -5850,7 +5849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>8</v>
       </c>
@@ -5861,7 +5860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>9</v>
       </c>
@@ -5872,7 +5871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>11</v>
       </c>
@@ -5883,7 +5882,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>12</v>
       </c>
@@ -5891,7 +5890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>13</v>
       </c>
@@ -5918,7 +5917,7 @@
       </c>
       <c r="I246" s="4"/>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247" t="str">
         <f>B237</f>
         <v>pipes assembly, for VRFB system</v>
@@ -5944,7 +5943,7 @@
       <c r="K247" s="3"/>
       <c r="L247" s="3"/>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>186</v>
       </c>
@@ -5971,7 +5970,7 @@
       <c r="K248" s="3"/>
       <c r="L248" s="3"/>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>309</v>
       </c>
@@ -5998,7 +5997,7 @@
       <c r="K249" s="3"/>
       <c r="L249" s="3"/>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
         <v>187</v>
       </c>
@@ -6025,7 +6024,7 @@
       <c r="K250" s="3"/>
       <c r="L250" s="3"/>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>344</v>
       </c>
@@ -6052,7 +6051,7 @@
       <c r="K251" s="3"/>
       <c r="L251" s="3"/>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>286</v>
       </c>
@@ -6076,13 +6075,13 @@
       </c>
       <c r="I252" s="4"/>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I253" s="3"/>
       <c r="J253" s="3"/>
       <c r="K253" s="3"/>
       <c r="L253" s="3"/>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>1</v>
       </c>
@@ -6093,7 +6092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>3</v>
       </c>
@@ -6104,7 +6103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>5</v>
       </c>
@@ -6115,7 +6114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>6</v>
       </c>
@@ -6123,7 +6122,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>7</v>
       </c>
@@ -6131,7 +6130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>8</v>
       </c>
@@ -6142,7 +6141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>9</v>
       </c>
@@ -6153,7 +6152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>11</v>
       </c>
@@ -6164,7 +6163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
         <v>12</v>
       </c>
@@ -6172,7 +6171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
         <v>13</v>
       </c>
@@ -6199,7 +6198,7 @@
       </c>
       <c r="I263" s="4"/>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A264" t="str">
         <f>B254</f>
         <v>heat exchanger production, for VRFB system</v>
@@ -6225,7 +6224,7 @@
       <c r="K264" s="3"/>
       <c r="L264" s="3"/>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>359</v>
       </c>
@@ -6248,7 +6247,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
         <v>193</v>
       </c>
@@ -6271,7 +6270,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>358</v>
       </c>
@@ -6295,7 +6294,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>282</v>
       </c>
@@ -6318,7 +6317,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>344</v>
       </c>
@@ -6341,7 +6340,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>286</v>
       </c>
@@ -6364,7 +6363,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
         <v>1</v>
       </c>
@@ -6375,7 +6374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>3</v>
       </c>
@@ -6386,7 +6385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>5</v>
       </c>
@@ -6397,7 +6396,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>6</v>
       </c>
@@ -6405,7 +6404,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>7</v>
       </c>
@@ -6413,7 +6412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>8</v>
       </c>
@@ -6424,7 +6423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>9</v>
       </c>
@@ -6435,7 +6434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>11</v>
       </c>
@@ -6446,7 +6445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
         <v>12</v>
       </c>
@@ -6454,7 +6453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
         <v>13</v>
       </c>
@@ -6481,7 +6480,7 @@
       </c>
       <c r="I281" s="4"/>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A282" t="str">
         <f>B272</f>
         <v>stack monitoring interface assembly, for VRFB system</v>
@@ -6507,7 +6506,7 @@
       <c r="K282" s="3"/>
       <c r="L282" s="3"/>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
         <v>109</v>
       </c>
@@ -6530,7 +6529,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
         <v>206</v>
       </c>
@@ -6553,7 +6552,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
         <v>207</v>
       </c>
@@ -6576,7 +6575,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
         <v>208</v>
       </c>
@@ -6599,7 +6598,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
         <v>210</v>
       </c>
@@ -6622,7 +6621,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
         <v>209</v>
       </c>
@@ -6645,7 +6644,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
         <v>294</v>
       </c>
@@ -6668,7 +6667,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
         <v>344</v>
       </c>
@@ -6691,7 +6690,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
         <v>286</v>
       </c>
@@ -6714,10 +6713,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H292" s="4"/>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
         <v>1</v>
       </c>
@@ -6728,7 +6727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>3</v>
       </c>
@@ -6739,7 +6738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>5</v>
       </c>
@@ -6750,7 +6749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>6</v>
       </c>
@@ -6758,7 +6757,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>7</v>
       </c>
@@ -6766,7 +6765,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>8</v>
       </c>
@@ -6777,7 +6776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>9</v>
       </c>
@@ -6788,7 +6787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>11</v>
       </c>
@@ -6799,7 +6798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
         <v>12</v>
       </c>
@@ -6807,7 +6806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
         <v>13</v>
       </c>
@@ -6834,7 +6833,7 @@
       </c>
       <c r="I302" s="4"/>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A303" t="str">
         <f>B293</f>
         <v>battery management system assembly, for VRFB system</v>
@@ -6860,7 +6859,7 @@
       <c r="K303" s="3"/>
       <c r="L303" s="3"/>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
         <v>210</v>
       </c>
@@ -6883,7 +6882,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
         <v>294</v>
       </c>
@@ -6906,7 +6905,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
         <v>222</v>
       </c>
@@ -6929,7 +6928,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
         <v>223</v>
       </c>
@@ -6952,7 +6951,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
         <v>344</v>
       </c>
@@ -6975,7 +6974,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
         <v>286</v>
       </c>
@@ -6998,7 +6997,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
         <v>1</v>
       </c>
@@ -7009,7 +7008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>3</v>
       </c>
@@ -7020,7 +7019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>5</v>
       </c>
@@ -7031,7 +7030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>6</v>
       </c>
@@ -7039,7 +7038,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>7</v>
       </c>
@@ -7047,7 +7046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>8</v>
       </c>
@@ -7058,7 +7057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>9</v>
       </c>
@@ -7069,7 +7068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>11</v>
       </c>
@@ -7080,7 +7079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
         <v>12</v>
       </c>
@@ -7088,7 +7087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
         <v>13</v>
       </c>
@@ -7115,7 +7114,7 @@
       </c>
       <c r="I320" s="4"/>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A321" t="str">
         <f>B311</f>
         <v>process control system assembly, for VRFB system</v>
@@ -7141,7 +7140,7 @@
       <c r="K321" s="3"/>
       <c r="L321" s="3"/>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>196</v>
       </c>
@@ -7165,7 +7164,7 @@
       </c>
       <c r="L322" s="3"/>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>216</v>
       </c>
@@ -7189,7 +7188,7 @@
       </c>
       <c r="L323" s="3"/>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
         <v>1</v>
       </c>
@@ -7200,7 +7199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>3</v>
       </c>
@@ -7211,7 +7210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>5</v>
       </c>
@@ -7222,7 +7221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>7</v>
       </c>
@@ -7230,7 +7229,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>8</v>
       </c>
@@ -7241,7 +7240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>9</v>
       </c>
@@ -7252,7 +7251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>11</v>
       </c>
@@ -7263,7 +7262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A332" s="1" t="s">
         <v>12</v>
       </c>
@@ -7271,7 +7270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A333" s="1" t="s">
         <v>13</v>
       </c>
@@ -7298,7 +7297,7 @@
       </c>
       <c r="I333" s="4"/>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A334" t="str">
         <f>B325</f>
         <v>treatment of stack, for VRFB system</v>
@@ -7324,7 +7323,7 @@
       <c r="K334" s="3"/>
       <c r="L334" s="3"/>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>307</v>
       </c>
@@ -7344,7 +7343,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>306</v>
       </c>
@@ -7364,7 +7363,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>304</v>
       </c>
@@ -7384,7 +7383,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>302</v>
       </c>
@@ -7404,7 +7403,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>301</v>
       </c>
@@ -7424,7 +7423,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>232</v>
       </c>
@@ -7444,7 +7443,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>234</v>
       </c>
@@ -7464,7 +7463,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A343" s="1" t="s">
         <v>1</v>
       </c>
@@ -7475,7 +7474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>3</v>
       </c>
@@ -7486,7 +7485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>5</v>
       </c>
@@ -7497,7 +7496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>7</v>
       </c>
@@ -7505,7 +7504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>8</v>
       </c>
@@ -7516,7 +7515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>9</v>
       </c>
@@ -7527,7 +7526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>11</v>
       </c>
@@ -7538,7 +7537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A350" s="1" t="s">
         <v>12</v>
       </c>
@@ -7546,7 +7545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A351" s="1" t="s">
         <v>13</v>
       </c>
@@ -7573,7 +7572,7 @@
       </c>
       <c r="I351" s="4"/>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A352" t="str">
         <f>B343</f>
         <v>treatment of electrolyte tank, for VRFB system</v>
@@ -7599,7 +7598,7 @@
       <c r="K352" s="3"/>
       <c r="L352" s="3"/>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>232</v>
       </c>
@@ -7619,7 +7618,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A354" s="3" t="s">
         <v>344</v>
       </c>
@@ -7642,7 +7641,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>306</v>
       </c>
@@ -7662,7 +7661,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
         <v>1</v>
       </c>
@@ -7673,7 +7672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>3</v>
       </c>
@@ -7684,7 +7683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>5</v>
       </c>
@@ -7695,7 +7694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>7</v>
       </c>
@@ -7703,7 +7702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>8</v>
       </c>
@@ -7714,7 +7713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>9</v>
       </c>
@@ -7725,7 +7724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>11</v>
       </c>
@@ -7736,7 +7735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
         <v>12</v>
       </c>
@@ -7744,7 +7743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A365" s="1" t="s">
         <v>13</v>
       </c>
@@ -7771,7 +7770,7 @@
       </c>
       <c r="I365" s="4"/>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A366" t="str">
         <f>B357</f>
         <v>treatment of electrolyte solution, for VRFB system</v>
@@ -7797,7 +7796,7 @@
       <c r="K366" s="3"/>
       <c r="L366" s="3"/>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>232</v>
       </c>
@@ -7817,7 +7816,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A368" s="3" t="s">
         <v>344</v>
       </c>
@@ -7840,7 +7839,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="370" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
         <v>1</v>
       </c>
@@ -7851,7 +7850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="371" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>3</v>
       </c>
@@ -7862,7 +7861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="372" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>5</v>
       </c>
@@ -7873,7 +7872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="373" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>7</v>
       </c>
@@ -7881,7 +7880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="374" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>8</v>
       </c>
@@ -7892,7 +7891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="375" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>9</v>
       </c>
@@ -7903,7 +7902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="376" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>11</v>
       </c>
@@ -7914,7 +7913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="377" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A377" s="1" t="s">
         <v>12</v>
       </c>
@@ -7922,7 +7921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="378" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
         <v>13</v>
       </c>
@@ -7949,7 +7948,7 @@
       </c>
       <c r="I378" s="4"/>
     </row>
-    <row r="379" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A379" t="str">
         <f>B370</f>
         <v>treatment of periphericals, for VRFB system</v>
@@ -7977,7 +7976,7 @@
       <c r="M379" s="3"/>
       <c r="N379" s="3"/>
     </row>
-    <row r="380" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>232</v>
       </c>
@@ -8001,7 +8000,7 @@
       <c r="M380" s="3"/>
       <c r="N380" s="3"/>
     </row>
-    <row r="381" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>234</v>
       </c>
@@ -8025,7 +8024,7 @@
       <c r="M381" s="3"/>
       <c r="N381" s="3"/>
     </row>
-    <row r="382" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>302</v>
       </c>
@@ -8046,7 +8045,7 @@
       </c>
       <c r="K382" s="4"/>
     </row>
-    <row r="383" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>243</v>
       </c>
@@ -8070,7 +8069,7 @@
       <c r="M383" s="3"/>
       <c r="N383" s="3"/>
     </row>
-    <row r="384" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>245</v>
       </c>
@@ -8094,7 +8093,7 @@
       <c r="M384" s="3"/>
       <c r="N384" s="3"/>
     </row>
-    <row r="385" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>306</v>
       </c>
@@ -8118,13 +8117,13 @@
       <c r="M385" s="3"/>
       <c r="N385" s="3"/>
     </row>
-    <row r="386" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:16" x14ac:dyDescent="0.2">
       <c r="K386" s="3"/>
       <c r="L386" s="3"/>
       <c r="M386" s="3"/>
       <c r="N386" s="3"/>
     </row>
-    <row r="387" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A387" s="1" t="s">
         <v>1</v>
       </c>
@@ -8135,7 +8134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="388" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>3</v>
       </c>
@@ -8146,7 +8145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="389" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>6</v>
       </c>
@@ -8154,7 +8153,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="390" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>5</v>
       </c>
@@ -8165,7 +8164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="391" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>7</v>
       </c>
@@ -8173,7 +8172,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="392" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>8</v>
       </c>
@@ -8184,7 +8183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="393" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>9</v>
       </c>
@@ -8195,7 +8194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="394" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>11</v>
       </c>
@@ -8206,7 +8205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="395" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A395" s="1" t="s">
         <v>12</v>
       </c>
@@ -8214,7 +8213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="396" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
         <v>13</v>
       </c>
@@ -8241,7 +8240,7 @@
       </c>
       <c r="I396" s="4"/>
     </row>
-    <row r="397" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A397" t="str">
         <f>B387</f>
         <v>vanadium-redox flow battery stack assembly</v>
@@ -8270,7 +8269,7 @@
       <c r="M397" s="3"/>
       <c r="N397" s="3"/>
     </row>
-    <row r="398" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>18</v>
       </c>
@@ -8301,7 +8300,7 @@
       <c r="O398" s="2"/>
       <c r="P398" s="2"/>
     </row>
-    <row r="399" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>67</v>
       </c>
@@ -8330,7 +8329,7 @@
       <c r="N399" s="3"/>
       <c r="O399" s="3"/>
     </row>
-    <row r="400" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>363</v>
       </c>
@@ -8359,7 +8358,7 @@
       <c r="N400" s="3"/>
       <c r="O400" s="3"/>
     </row>
-    <row r="401" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>135</v>
       </c>
@@ -8388,7 +8387,7 @@
       <c r="N401" s="3"/>
       <c r="O401" s="3"/>
     </row>
-    <row r="402" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>143</v>
       </c>
@@ -8417,7 +8416,7 @@
       <c r="N402" s="3"/>
       <c r="O402" s="3"/>
     </row>
-    <row r="403" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>148</v>
       </c>
@@ -8446,7 +8445,7 @@
       <c r="N403" s="3"/>
       <c r="O403" s="3"/>
     </row>
-    <row r="404" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>100</v>
       </c>
@@ -8475,7 +8474,7 @@
       <c r="N404" s="3"/>
       <c r="O404" s="3"/>
     </row>
-    <row r="405" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B405" s="3"/>
       <c r="H405" s="3"/>
       <c r="I405" s="3"/>
@@ -8485,7 +8484,7 @@
       <c r="N405" s="3"/>
       <c r="O405" s="3"/>
     </row>
-    <row r="406" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
         <v>1</v>
       </c>
@@ -8496,7 +8495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="407" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>3</v>
       </c>
@@ -8507,7 +8506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="408" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>6</v>
       </c>
@@ -8515,7 +8514,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="409" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>5</v>
       </c>
@@ -8526,7 +8525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="410" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>7</v>
       </c>
@@ -8534,7 +8533,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="411" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>8</v>
       </c>
@@ -8545,7 +8544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="412" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>9</v>
       </c>
@@ -8556,7 +8555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="413" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>11</v>
       </c>
@@ -8567,7 +8566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="414" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A414" s="1" t="s">
         <v>12</v>
       </c>
@@ -8575,7 +8574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="415" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A415" s="1" t="s">
         <v>13</v>
       </c>
@@ -8602,7 +8601,7 @@
       </c>
       <c r="I415" s="4"/>
     </row>
-    <row r="416" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A416" t="str">
         <f>B406</f>
         <v>vanadium-redox flow battery system assembly, 8.3 megawatt hour</v>
@@ -8631,7 +8630,7 @@
       <c r="M416" s="3"/>
       <c r="N416" s="3"/>
     </row>
-    <row r="417" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>265</v>
       </c>
@@ -8662,7 +8661,7 @@
       <c r="O417" s="2"/>
       <c r="P417" s="2"/>
     </row>
-    <row r="418" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>112</v>
       </c>
@@ -8691,7 +8690,7 @@
       <c r="N418" s="3"/>
       <c r="O418" s="3"/>
     </row>
-    <row r="419" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>134</v>
       </c>
@@ -8720,7 +8719,7 @@
       <c r="N419" s="3"/>
       <c r="O419" s="3"/>
     </row>
-    <row r="420" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>179</v>
       </c>
@@ -8749,7 +8748,7 @@
       <c r="N420" s="3"/>
       <c r="O420" s="3"/>
     </row>
-    <row r="421" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>169</v>
       </c>
@@ -8778,7 +8777,7 @@
       <c r="N421" s="3"/>
       <c r="O421" s="3"/>
     </row>
-    <row r="422" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>261</v>
       </c>
@@ -8807,7 +8806,7 @@
       <c r="N422" s="3"/>
       <c r="O422" s="3"/>
     </row>
-    <row r="423" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>162</v>
       </c>
@@ -8836,7 +8835,7 @@
       <c r="N423" s="3"/>
       <c r="O423" s="3"/>
     </row>
-    <row r="424" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>226</v>
       </c>
@@ -8865,7 +8864,7 @@
       <c r="N424" s="3"/>
       <c r="O424" s="3"/>
     </row>
-    <row r="425" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>195</v>
       </c>
@@ -8894,7 +8893,7 @@
       <c r="N425" s="3"/>
       <c r="O425" s="3"/>
     </row>
-    <row r="426" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I426" s="3"/>
       <c r="J426" s="3"/>
       <c r="K426" s="3"/>
@@ -8903,7 +8902,7 @@
       <c r="N426" s="3"/>
       <c r="O426" s="3"/>
     </row>
-    <row r="427" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A427" s="1" t="s">
         <v>1</v>
       </c>
@@ -8914,7 +8913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="428" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>3</v>
       </c>
@@ -8925,7 +8924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="429" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>6</v>
       </c>
@@ -8933,7 +8932,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="430" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>5</v>
       </c>
@@ -8944,7 +8943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="431" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>7</v>
       </c>
@@ -8952,7 +8951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="432" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>8</v>
       </c>
@@ -8963,7 +8962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="433" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>9</v>
       </c>
@@ -8974,7 +8973,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="434" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>11</v>
       </c>
@@ -8985,7 +8984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="435" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A435" s="1" t="s">
         <v>12</v>
       </c>
@@ -8993,7 +8992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="436" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A436" s="1" t="s">
         <v>13</v>
       </c>
@@ -9020,7 +9019,7 @@
       </c>
       <c r="I436" s="4"/>
     </row>
-    <row r="437" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A437" t="str">
         <f>B427</f>
         <v>electricity supply, high voltage, from vanadium-redox flow battery system</v>
@@ -9049,7 +9048,7 @@
       <c r="M437" s="3"/>
       <c r="N437" s="3"/>
     </row>
-    <row r="438" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>269</v>
       </c>
@@ -9078,7 +9077,7 @@
       <c r="M438" s="3"/>
       <c r="N438" s="3"/>
     </row>
-    <row r="439" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>264</v>
       </c>
@@ -9102,7 +9101,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="440" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>265</v>
       </c>
@@ -9126,7 +9125,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="441" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>230</v>
       </c>
@@ -9150,7 +9149,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="442" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>236</v>
       </c>
@@ -9174,7 +9173,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="443" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
         <v>238</v>
       </c>
@@ -9198,7 +9197,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="444" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
         <v>240</v>
       </c>
@@ -9222,7 +9221,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="446" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A446" s="1" t="s">
         <v>1</v>
       </c>
@@ -9230,7 +9229,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="447" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
         <v>3</v>
       </c>
@@ -9238,7 +9237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="448" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
         <v>6</v>
       </c>
@@ -9246,7 +9245,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="449" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>5</v>
       </c>
@@ -9254,7 +9253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="450" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>7</v>
       </c>
@@ -9262,7 +9261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="451" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>8</v>
       </c>
@@ -9270,7 +9269,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="452" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>9</v>
       </c>
@@ -9278,7 +9277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="453" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>11</v>
       </c>
@@ -9286,13 +9285,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="454" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A454" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I454" s="9"/>
     </row>
-    <row r="455" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A455" s="1" t="s">
         <v>13</v>
       </c>
@@ -9318,7 +9317,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="456" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A456" t="str">
         <f>B446</f>
         <v>market for battery, redox-flow, Vanadium</v>
@@ -9341,7 +9340,7 @@
         <v>battery, redox-flow, Vanadium</v>
       </c>
     </row>
-    <row r="457" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>264</v>
       </c>
@@ -9364,9 +9363,8 @@
       <c r="H457" t="s">
         <v>365</v>
       </c>
-      <c r="I457" s="10"/>
-    </row>
-    <row r="458" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="458" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>265</v>
       </c>
@@ -9388,10 +9386,10 @@
       </c>
       <c r="I458" s="9"/>
     </row>
-    <row r="459" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B459" s="9"/>
     </row>
-    <row r="461" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A461" s="1" t="s">
         <v>1</v>
       </c>
@@ -9399,7 +9397,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="462" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
         <v>3</v>
       </c>
@@ -9407,12 +9405,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="463" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="464" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
         <v>5</v>
       </c>
@@ -9420,7 +9418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="465" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
         <v>7</v>
       </c>
@@ -9428,7 +9426,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="466" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
         <v>8</v>
       </c>
@@ -9436,7 +9434,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
         <v>9</v>
       </c>
@@ -9444,7 +9442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="468" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>11</v>
       </c>
@@ -9452,12 +9450,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="469" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A469" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="470" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A470" s="1" t="s">
         <v>13</v>
       </c>
@@ -9483,13 +9481,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="471" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A471" t="str">
         <f>B461</f>
         <v>market for used redox-flow battery</v>
       </c>
       <c r="B471">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C471" t="s">
         <v>28</v>
@@ -9506,7 +9504,7 @@
         <v>used redox-flow battery</v>
       </c>
     </row>
-    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>230</v>
       </c>
@@ -9527,7 +9525,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="473" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
         <v>236</v>
       </c>
@@ -9548,7 +9546,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
         <v>238</v>
       </c>
@@ -9569,7 +9567,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="475" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
         <v>240</v>
       </c>

</xml_diff>